<commit_message>
added AF3 predictions of ligand MPNN sequences and updated filename reference excel for PAS-MES binding
</commit_message>
<xml_diff>
--- a/mes-binder/PAS-mes/mes_ligand_mpnn_filename_ref.xlsx
+++ b/mes-binder/PAS-mes/mes_ligand_mpnn_filename_ref.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wei_g\Desktop\Designs\mes-binder\PAS-mes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wei_g\Desktop\Designs\enzyme_engineering\mes-binder\PAS-mes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D75841F-5DA4-4B2B-BD98-35454254AEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E3FE2A-DE39-4FB6-A06A-A982E6447D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10095" yWindow="0" windowWidth="10410" windowHeight="10905" xr2:uid="{C934E24C-7FE0-4CA2-990A-91182BDDDE74}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{C934E24C-7FE0-4CA2-990A-91182BDDDE74}"/>
   </bookViews>
   <sheets>
-    <sheet name="for ligand MPNN" sheetId="1" r:id="rId1"/>
+    <sheet name="diffusion -&gt; protein mpnn -&gt; AF" sheetId="1" r:id="rId1"/>
+    <sheet name="ligand mpnn -&gt; AF3 -&gt; docking" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t>Original protein</t>
   </si>
@@ -39,9 +40,6 @@
     <t>protein MPNN seq id</t>
   </si>
   <si>
-    <t>Filename</t>
-  </si>
-  <si>
     <t>PAS</t>
   </si>
   <si>
@@ -70,6 +68,66 @@
   </si>
   <si>
     <t>residues within 8A changed</t>
+  </si>
+  <si>
+    <t>Ligand MPNN input filename</t>
+  </si>
+  <si>
+    <t>ligand MPNN seq id</t>
+  </si>
+  <si>
+    <t>AF3 project name</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>overall confidence</t>
+  </si>
+  <si>
+    <t>side chain packing</t>
+  </si>
+  <si>
+    <t>ligand mpnn parameters</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>ligand confidence</t>
+  </si>
+  <si>
+    <t>seq rec</t>
+  </si>
+  <si>
+    <t>higher temp 0.25</t>
+  </si>
+  <si>
+    <t>pas_mes_8A_lig_1</t>
+  </si>
+  <si>
+    <t>pas_mes_8A_lig_2</t>
+  </si>
+  <si>
+    <t>pas_mes_8A_lig_3</t>
+  </si>
+  <si>
+    <t>pas_mes_8A-2_lig_1</t>
+  </si>
+  <si>
+    <t>pas_mes_8A-2_lig_2</t>
+  </si>
+  <si>
+    <t>pas_mes_8A-2_lig_3</t>
+  </si>
+  <si>
+    <t>pas_mes_mpnn_lig_1</t>
+  </si>
+  <si>
+    <t>pas_mes_mpnn_lig_2</t>
+  </si>
+  <si>
+    <t>pas_mes_mpnn_lig_3</t>
   </si>
 </sst>
 </file>
@@ -92,12 +150,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -112,10 +176,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,17 +509,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A9FB470-8A86-4005-97EB-66EB0B37B6A1}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.85546875" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
   </cols>
@@ -454,40 +531,40 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
+      <c r="E1" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
+      <c r="E2" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" s="1">
         <v>45446</v>
@@ -495,22 +572,22 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>3</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
-        <v>11</v>
+      <c r="E3" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="1">
         <v>45446</v>
@@ -518,22 +595,22 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2">
         <v>7</v>
       </c>
-      <c r="D4">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="E4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
         <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
       </c>
       <c r="G4" s="1">
         <v>45446</v>
@@ -543,4 +620,288 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C50A9BD-57CF-43D4-93D1-88EF9B077C53}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.54300000000000004</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.6119</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="1">
+        <v>45447</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="2">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.52949999999999997</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.46710000000000002</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.6119</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="1">
+        <v>45447</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="2">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.50900000000000001</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.51390000000000002</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.62690000000000001</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="1">
+        <v>45447</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.50119999999999998</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.43059999999999998</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.62209999999999999</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="1">
+        <v>45447</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="2">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.49930000000000002</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.3916</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.61339999999999995</v>
+      </c>
+      <c r="G6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="1">
+        <v>45447</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="2">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.48580000000000001</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.40589999999999998</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.60470000000000002</v>
+      </c>
+      <c r="G7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="1">
+        <v>45447</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.55010000000000003</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.54830000000000001</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.68169999999999997</v>
+      </c>
+      <c r="G8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="1">
+        <v>45447</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="2">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.54159999999999997</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.5181</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.69369999999999998</v>
+      </c>
+      <c r="G9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="1">
+        <v>45447</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2">
+        <v>10</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.52900000000000003</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.47860000000000003</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.67869999999999997</v>
+      </c>
+      <c r="G10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="1">
+        <v>45447</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
removed unrelated files and added AF3 predictions for some ligand mpnn sequences
</commit_message>
<xml_diff>
--- a/mes-binder/PAS-mes/mes_ligand_mpnn_filename_ref.xlsx
+++ b/mes-binder/PAS-mes/mes_ligand_mpnn_filename_ref.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wei_g\Desktop\Designs\enzyme_engineering\mes-binder\PAS-mes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E3FE2A-DE39-4FB6-A06A-A982E6447D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E18CB8C-28BD-49B5-9617-9E4A6AB5F702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{C934E24C-7FE0-4CA2-990A-91182BDDDE74}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="10410" windowHeight="10905" firstSheet="1" activeTab="1" xr2:uid="{C934E24C-7FE0-4CA2-990A-91182BDDDE74}"/>
   </bookViews>
   <sheets>
     <sheet name="diffusion -&gt; protein mpnn -&gt; AF" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
   <si>
     <t>Original protein</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>pas_mes_mpnn_lig_3</t>
+  </si>
+  <si>
+    <t>ligand score</t>
   </si>
 </sst>
 </file>
@@ -176,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -186,11 +189,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -507,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A9FB470-8A86-4005-97EB-66EB0B37B6A1}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,12 +518,13 @@
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
     <col min="3" max="3" width="25.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.85546875" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="5" max="7" width="19.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="27.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.85546875" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -537,17 +537,26 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -560,17 +569,26 @@
       <c r="D2" s="2">
         <v>3</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="2">
+        <v>0.40350000000000003</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.40350000000000003</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.31940000000000002</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="1">
+      <c r="J2" s="1">
         <v>45446</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -583,17 +601,26 @@
       <c r="D3" s="2">
         <v>5</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="2">
+        <v>0.43209999999999998</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.43209999999999998</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.36630000000000001</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="1">
+      <c r="J3" s="1">
         <v>45446</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -606,13 +633,22 @@
       <c r="D4" s="2">
         <v>7</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="2">
+        <v>0.45250000000000001</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.45250000000000001</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.45950000000000002</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F4" t="s">
+      <c r="I4" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="1">
+      <c r="J4" s="1">
         <v>45446</v>
       </c>
     </row>
@@ -626,7 +662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C50A9BD-57CF-43D4-93D1-88EF9B077C53}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -669,7 +705,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
@@ -695,7 +731,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
+      <c r="A3" s="5"/>
       <c r="B3" t="s">
         <v>19</v>
       </c>
@@ -719,7 +755,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
+      <c r="A4" s="5"/>
       <c r="B4" t="s">
         <v>24</v>
       </c>
@@ -743,7 +779,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
@@ -769,7 +805,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+      <c r="A6" s="5"/>
       <c r="B6" t="s">
         <v>19</v>
       </c>
@@ -793,7 +829,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
+      <c r="A7" s="5"/>
       <c r="B7" t="s">
         <v>24</v>
       </c>
@@ -817,7 +853,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
@@ -843,7 +879,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="5"/>
       <c r="B9" t="s">
         <v>19</v>
       </c>
@@ -867,7 +903,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="5"/>
       <c r="B10" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
docking results for pas-mes binding
</commit_message>
<xml_diff>
--- a/mes-binder/PAS-mes/mes_ligand_mpnn_filename_ref.xlsx
+++ b/mes-binder/PAS-mes/mes_ligand_mpnn_filename_ref.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wei_g\Desktop\Designs\enzyme_engineering\mes-binder\PAS-mes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wei_g\Desktop\Designs\mes-binder\PAS-mes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E18CB8C-28BD-49B5-9617-9E4A6AB5F702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E79E87C-250F-41ED-B34D-0E64A8C6D993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="10410" windowHeight="10905" firstSheet="1" activeTab="1" xr2:uid="{C934E24C-7FE0-4CA2-990A-91182BDDDE74}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{C934E24C-7FE0-4CA2-990A-91182BDDDE74}"/>
   </bookViews>
   <sheets>
     <sheet name="diffusion -&gt; protein mpnn -&gt; AF" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
   <si>
     <t>Original protein</t>
   </si>
@@ -131,6 +131,12 @@
   </si>
   <si>
     <t>ligand score</t>
+  </si>
+  <si>
+    <t>Docking affinity (best model autodock vina)</t>
+  </si>
+  <si>
+    <t>Rejected, steric clash with substrate</t>
   </si>
 </sst>
 </file>
@@ -153,7 +159,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -163,6 +169,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -179,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -191,6 +203,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -508,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A9FB470-8A86-4005-97EB-66EB0B37B6A1}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,10 +678,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C50A9BD-57CF-43D4-93D1-88EF9B077C53}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,9 +694,10 @@
     <col min="6" max="6" width="18.42578125" customWidth="1"/>
     <col min="7" max="7" width="23.28515625" customWidth="1"/>
     <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="44.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
@@ -703,8 +722,14 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
@@ -729,8 +754,14 @@
       <c r="H2" s="1">
         <v>45447</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="7">
+        <v>-9.0190000000000001</v>
+      </c>
+      <c r="J2" s="1">
+        <v>45448</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" t="s">
         <v>19</v>
@@ -753,8 +784,14 @@
       <c r="H3" s="1">
         <v>45447</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="2">
+        <v>-8.798</v>
+      </c>
+      <c r="J3" s="1">
+        <v>45448</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" t="s">
         <v>24</v>
@@ -777,9 +814,15 @@
       <c r="H4" s="1">
         <v>45447</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="I4" s="2">
+        <v>-9.5589999999999993</v>
+      </c>
+      <c r="J4" s="1">
+        <v>45448</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
@@ -803,9 +846,15 @@
       <c r="H5" s="1">
         <v>45447</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
+      <c r="I5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="1">
+        <v>45448</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
       <c r="B6" t="s">
         <v>19</v>
       </c>
@@ -827,9 +876,15 @@
       <c r="H6" s="1">
         <v>45447</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
+      <c r="I6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" s="1">
+        <v>45448</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
       <c r="B7" t="s">
         <v>24</v>
       </c>
@@ -851,8 +906,14 @@
       <c r="H7" s="1">
         <v>45447</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" s="1">
+        <v>45448</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>11</v>
       </c>
@@ -877,8 +938,14 @@
       <c r="H8" s="1">
         <v>45447</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="2">
+        <v>-9.2680000000000007</v>
+      </c>
+      <c r="J8" s="1">
+        <v>45448</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" t="s">
         <v>19</v>
@@ -901,8 +968,14 @@
       <c r="H9" s="1">
         <v>45447</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="2">
+        <v>-8.34</v>
+      </c>
+      <c r="J9" s="1">
+        <v>45448</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" t="s">
         <v>24</v>
@@ -925,8 +998,14 @@
       <c r="H10" s="1">
         <v>45447</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="2">
+        <v>-9.2609999999999992</v>
+      </c>
+      <c r="J10" s="1">
+        <v>45448</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -939,5 +1018,6 @@
     <mergeCell ref="A8:A10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
final docking results. Added a pse file with lzx suggestions for mutations and a to do file.
</commit_message>
<xml_diff>
--- a/mes-binder/PAS-mes/mes_ligand_mpnn_filename_ref.xlsx
+++ b/mes-binder/PAS-mes/mes_ligand_mpnn_filename_ref.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wei_g\Desktop\Designs\mes-binder\PAS-mes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2ABD94-D80D-4EB5-9C40-0299E7C65A1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF211B4-ADD7-4552-9CB6-CA7C989091A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="1110" windowWidth="21675" windowHeight="17130" activeTab="1" xr2:uid="{C934E24C-7FE0-4CA2-990A-91182BDDDE74}"/>
+    <workbookView xWindow="7485" yWindow="3030" windowWidth="26205" windowHeight="17130" xr2:uid="{C934E24C-7FE0-4CA2-990A-91182BDDDE74}"/>
   </bookViews>
   <sheets>
     <sheet name="diffusion -&gt; protein mpnn -&gt; AF" sheetId="1" r:id="rId1"/>
@@ -191,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -207,6 +207,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,7 +524,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A9FB470-8A86-4005-97EB-66EB0B37B6A1}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -677,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C50A9BD-57CF-43D4-93D1-88EF9B077C53}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,7 +731,7 @@
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="2">
@@ -760,7 +761,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="2">
@@ -790,7 +791,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C4" s="2">
@@ -822,7 +823,7 @@
       <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="2">
@@ -852,7 +853,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
-      <c r="B6" t="s">
+      <c r="B6" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="2">
@@ -882,7 +883,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
-      <c r="B7" t="s">
+      <c r="B7" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C7" s="2">
@@ -914,7 +915,7 @@
       <c r="A8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="2">
@@ -944,7 +945,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="2">
@@ -974,7 +975,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C10" s="2">

</xml_diff>